<commit_message>
updated supplemental table to use mean expression and renaming
</commit_message>
<xml_diff>
--- a/Resubmission_Figures/Supplemental_Table/table_column_mappings.xlsx
+++ b/Resubmission_Figures/Supplemental_Table/table_column_mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnz/Documents/GitFiles/discordant-transcript-resubmission/Resubmission_Figures/Supplemental_Table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DC68CF-1F0A-F045-B151-7660AE41D0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9530E2-7779-194F-8852-8AD8B66D1B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{05F638F8-6F5B-AB44-B77A-D32928D1161A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16460" xr2:uid="{05F638F8-6F5B-AB44-B77A-D32928D1161A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>column</t>
   </si>
@@ -44,12 +44,6 @@
     <t>transcript_id</t>
   </si>
   <si>
-    <t>Tsoi_gene_spearman</t>
-  </si>
-  <si>
-    <t>Tsoi_gene_pearson</t>
-  </si>
-  <si>
     <t>Change prjna_overexpression to “PRJNA704810_OE MITF/CON”</t>
   </si>
   <si>
@@ -98,30 +92,6 @@
     <t>ccle_gene_pearson</t>
   </si>
   <si>
-    <t>tsoi_gene_spearman</t>
-  </si>
-  <si>
-    <t>tsoi_gene_pearson</t>
-  </si>
-  <si>
-    <t>prjna704810_oe mitf/con</t>
-  </si>
-  <si>
-    <t>gse_163646_oe mitf/con</t>
-  </si>
-  <si>
-    <t>prjeb30337_sicon/simitf</t>
-  </si>
-  <si>
-    <t>gse163646_sicon/simitf</t>
-  </si>
-  <si>
-    <t>gse283655_sicon/simitf</t>
-  </si>
-  <si>
-    <t>gse115845_sicon/simitf</t>
-  </si>
-  <si>
     <t>has_peak_gse153020_kenny</t>
   </si>
   <si>
@@ -131,18 +101,6 @@
     <t>has_peak_gse77437_louph</t>
   </si>
   <si>
-    <t>ccle_median_transcript_expression</t>
-  </si>
-  <si>
-    <t>tsoi_median transcript expression</t>
-  </si>
-  <si>
-    <t>ccle_median gene expression</t>
-  </si>
-  <si>
-    <t>tsoi_median gene expression</t>
-  </si>
-  <si>
     <t>gene_id</t>
   </si>
   <si>
@@ -170,58 +128,76 @@
     <t>CCLE_gene_pearson to MITF expression</t>
   </si>
   <si>
-    <t>Median expression of the transcript based on CCLE data</t>
-  </si>
-  <si>
-    <t>Median expression of the transcript based on Tsoi data</t>
-  </si>
-  <si>
-    <t>Median expression of associated gene based on CCLE data</t>
-  </si>
-  <si>
-    <t>Median expression of associated gene based on Tsoi data</t>
-  </si>
-  <si>
-    <t>ccle_median_transcript_expression_mitf_high</t>
-  </si>
-  <si>
-    <t>tsoi_median transcript expression_mitf_high</t>
-  </si>
-  <si>
-    <t>ccle_median gene expression_mitf_high</t>
-  </si>
-  <si>
-    <t>tsoi_median gene expression_mitf_high</t>
-  </si>
-  <si>
-    <t>Median expression of the transcript based on CCLE data in high-MITF expressing cell-lines ONLY</t>
-  </si>
-  <si>
-    <t>Median expression of the transcript based on Tsoi data in high-MITF expressing cell-lines ONLY</t>
-  </si>
-  <si>
-    <t>Median expression of associated gene based on CCLE data in high-MITF expressing cell-lines ONLY</t>
-  </si>
-  <si>
-    <t>Median expression of associated gene based on Tsoi data in high-MITF expressing cell-lines ONLY</t>
-  </si>
-  <si>
     <t>ebox_n</t>
   </si>
   <si>
     <t xml:space="preserve">Number of eboxes, using data from Figure 2 </t>
   </si>
   <si>
-    <t>&lt;- These median expression values are slightly different from Supplemental Figure 4. Because in Suppplementary-4, we are looking at the log2_mean+1 of expression for each transcript.</t>
-  </si>
-  <si>
-    <t>But for this metric, we are looking at the median expression.</t>
-  </si>
-  <si>
-    <t>&lt;- do we need this, we didn't  use this in the analysis</t>
-  </si>
-  <si>
-    <t>Also for supplemnetary-4, I think we only used CCLE data</t>
+    <t>ccle_mean_transcript_expression</t>
+  </si>
+  <si>
+    <t>tsoi_mean transcript expression</t>
+  </si>
+  <si>
+    <t>ccle_mean gene expression</t>
+  </si>
+  <si>
+    <t>tsoi_mean gene expression</t>
+  </si>
+  <si>
+    <t>ccle_mean_transcript_expression_mitf_high</t>
+  </si>
+  <si>
+    <t>tsoi_mean transcript expression_mitf_high</t>
+  </si>
+  <si>
+    <t>ccle_mean gene expression_mitf_high</t>
+  </si>
+  <si>
+    <t>tsoi_mean gene expression_mitf_high</t>
+  </si>
+  <si>
+    <t>Mean expression of the transcript based on CCLE data</t>
+  </si>
+  <si>
+    <t>Mean expression of the transcript based on Tsoi data</t>
+  </si>
+  <si>
+    <t>Mean expression of associated gene based on CCLE data</t>
+  </si>
+  <si>
+    <t>Mean expression of associated gene based on Tsoi data</t>
+  </si>
+  <si>
+    <t>Mean expression of the transcript based on CCLE data in high-MITF expressing cell-lines ONLY</t>
+  </si>
+  <si>
+    <t>Mean expression of the transcript based on Tsoi data in high-MITF expressing cell-lines ONLY</t>
+  </si>
+  <si>
+    <t>Mean expression of associated gene based on CCLE data in high-MITF expressing cell-lines ONLY</t>
+  </si>
+  <si>
+    <t>Mean expression of associated gene based on Tsoi data in high-MITF expressing cell-lines ONLY</t>
+  </si>
+  <si>
+    <t>PRJNA704810_OE_MITF/CON</t>
+  </si>
+  <si>
+    <t>GSE163646_OE_MITF/CON</t>
+  </si>
+  <si>
+    <t>PRJEB30337_siCON/siMITF</t>
+  </si>
+  <si>
+    <t>GSE163646_siCON/siMITF</t>
+  </si>
+  <si>
+    <t>GSE283655_siCON/siMITF</t>
+  </si>
+  <si>
+    <t>GSE115845_siCON/siMITF</t>
   </si>
 </sst>
 </file>
@@ -249,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,12 +235,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,11 +590,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6FC45B-4741-C248-A7EA-2FC083EC099C}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,15 +603,15 @@
     <col min="2" max="2" width="88.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -649,181 +619,166 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>50</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
+      <c r="A21" t="s">
+        <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>24</v>
+      <c r="A22" t="s">
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>25</v>
+      <c r="A23" t="s">
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
@@ -831,7 +786,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -839,7 +794,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -847,7 +802,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>10</v>
@@ -855,36 +810,20 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>